<commit_message>
vnv - unit tests docs
</commit_message>
<xml_diff>
--- a/docs/VnVReport/test-analysis/metric_results_analysis.xlsx
+++ b/docs/VnVReport/test-analysis/metric_results_analysis.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joedf\Documents\GitHub\CAS741_w23\docs\VnVReport\test-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3757F16E-416C-4D85-A5DF-2DBA279E5D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EF94F2-8ADB-4A75-A8E5-6DC126E915F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15733" xr2:uid="{5B20B560-2675-4915-B90A-97D8720C64BF}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15733" activeTab="2" xr2:uid="{5B20B560-2675-4915-B90A-97D8720C64BF}"/>
   </bookViews>
   <sheets>
     <sheet name="js_tests" sheetId="1" r:id="rId1"/>
     <sheet name="py_tests" sheetId="2" r:id="rId2"/>
+    <sheet name="Ranks" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="71">
   <si>
     <t>testname</t>
   </si>
@@ -235,6 +236,21 @@
   </si>
   <si>
     <t>total time (ms)</t>
+  </si>
+  <si>
+    <t>MSE based metrics</t>
+  </si>
+  <si>
+    <t>SSIM based metrics</t>
+  </si>
+  <si>
+    <t>javascript tests</t>
+  </si>
+  <si>
+    <t>Python (sewar) tests</t>
+  </si>
+  <si>
+    <t>ms-ssim</t>
   </si>
 </sst>
 </file>
@@ -244,7 +260,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,16 +268,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -269,21 +307,289 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
@@ -370,19 +676,19 @@
     <tableColumn id="1" xr3:uid="{9611E537-4FE5-4C2D-9563-28B4D98E46B1}" name="#"/>
     <tableColumn id="2" xr3:uid="{F4267E20-0B79-4BB1-9ED6-D1F2798542E5}" name="testname"/>
     <tableColumn id="3" xr3:uid="{667F5C2D-228D-46C1-BF1E-AB83553AA98F}" name="Expected Rank"/>
-    <tableColumn id="4" xr3:uid="{A9B1C654-46D5-4D47-A59D-62A25EA835D9}" name="ssim (obartra)" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{27447F7F-34C1-450D-B649-BCD291EC9D27}" name="ssim (darosh)" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{BA47D22F-0BBA-4283-ADCA-CC3CFE1E00CC}" name="mse (jdf)" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{9B189C05-7059-4C40-B98C-AE4D4F0028F6}" name="psnr (jdf)" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{3B3AD642-EF8B-4A91-AE92-473ADB0DB518}" name="rmse (jdf)" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{B3BD767A-29A9-4F0D-B199-284EA05BA820}" name="nrmse (jdf)" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{E411ECA4-67A6-4CDA-9DC6-62CC7BCB1ED7}" name="inrmse (jdf)" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{A3FF7C39-6883-4E46-B55D-AC2F71D6EACF}" name="nmse (jdf)" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{E1B8E126-AA92-44F1-8714-BB56F7585F25}" name="inmse (jdf)" dataDxfId="12"/>
-    <tableColumn id="13" xr3:uid="{C6C61EA8-C8B6-4697-9BE2-F7E000E16A25}" name="mse (darosh)" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{9E237621-BCB6-4CD4-81F6-A4086220EAF0}" name="psnr (darosh)" dataDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{926C9206-BF6F-428E-9487-F8F4288AA3D0}" name="msssim (darosh)" dataDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{7BC4D969-0313-4FC7-9DDF-FAB4C8AB41AD}" name="ssim (darosh msssim)" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{A9B1C654-46D5-4D47-A59D-62A25EA835D9}" name="ssim (obartra)" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{27447F7F-34C1-450D-B649-BCD291EC9D27}" name="ssim (darosh)" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{BA47D22F-0BBA-4283-ADCA-CC3CFE1E00CC}" name="mse (jdf)" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{9B189C05-7059-4C40-B98C-AE4D4F0028F6}" name="psnr (jdf)" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{3B3AD642-EF8B-4A91-AE92-473ADB0DB518}" name="rmse (jdf)" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{B3BD767A-29A9-4F0D-B199-284EA05BA820}" name="nrmse (jdf)" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{E411ECA4-67A6-4CDA-9DC6-62CC7BCB1ED7}" name="inrmse (jdf)" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{A3FF7C39-6883-4E46-B55D-AC2F71D6EACF}" name="nmse (jdf)" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{E1B8E126-AA92-44F1-8714-BB56F7585F25}" name="inmse (jdf)" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{C6C61EA8-C8B6-4697-9BE2-F7E000E16A25}" name="mse (darosh)" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{9E237621-BCB6-4CD4-81F6-A4086220EAF0}" name="psnr (darosh)" dataDxfId="17"/>
+    <tableColumn id="15" xr3:uid="{926C9206-BF6F-428E-9487-F8F4288AA3D0}" name="msssim (darosh)" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{7BC4D969-0313-4FC7-9DDF-FAB4C8AB41AD}" name="ssim (darosh msssim)" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -398,14 +704,14 @@
     <tableColumn id="1" xr3:uid="{F7FE2A69-0D8E-49C4-80D3-BF8C23D0A027}" name="#"/>
     <tableColumn id="2" xr3:uid="{E2042B5B-9F31-463B-B5E0-4E2BBE1367F2}" name="testname"/>
     <tableColumn id="3" xr3:uid="{A3B370FA-A8E4-46C6-9439-A63E81737EFA}" name="Expected rank"/>
-    <tableColumn id="4" xr3:uid="{48C3E892-DFED-4EE2-A0D8-6306DCA34237}" name="mse" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{7CE22FCF-DC21-4054-8A35-B2C1101FA1C8}" name="rmse" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{5AE8EBCB-89A9-4705-A221-32289F3AFAEC}" name="psnr" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{861346B0-7E61-45D5-9D7E-1D21897B881E}" name="uqi" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{F5BCC34F-D45E-4B6D-BC5A-31FC723553B1}" name="ssim" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{4FB8FA19-043E-49A7-9018-53C3A3D83C08}" name="msssim" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{511E004F-6D7D-4886-BD9F-7CDCD82D3998}" name="scc" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{2C7229B4-3D0C-489A-BD8D-4436AC33D976}" name="vifp" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{48C3E892-DFED-4EE2-A0D8-6306DCA34237}" name="mse" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{7CE22FCF-DC21-4054-8A35-B2C1101FA1C8}" name="rmse" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{5AE8EBCB-89A9-4705-A221-32289F3AFAEC}" name="psnr" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{861346B0-7E61-45D5-9D7E-1D21897B881E}" name="uqi" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{F5BCC34F-D45E-4B6D-BC5A-31FC723553B1}" name="ssim" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{4FB8FA19-043E-49A7-9018-53C3A3D83C08}" name="msssim" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{511E004F-6D7D-4886-BD9F-7CDCD82D3998}" name="scc" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{2C7229B4-3D0C-489A-BD8D-4436AC33D976}" name="vifp" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -710,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B92C74-347A-4EDB-A0CE-4F0C99A5E60F}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1938,7 +2244,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D12">
-    <cfRule type="dataBar" priority="25">
+    <cfRule type="dataBar" priority="27">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1952,7 +2258,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:D24">
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1966,7 +2272,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E12">
-    <cfRule type="dataBar" priority="26">
+    <cfRule type="dataBar" priority="28">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1980,7 +2286,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:E24">
-    <cfRule type="dataBar" priority="12">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1994,7 +2300,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F12">
-    <cfRule type="dataBar" priority="24">
+    <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2008,7 +2314,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:F24">
-    <cfRule type="dataBar" priority="11">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2022,7 +2328,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G12">
-    <cfRule type="dataBar" priority="23">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2036,7 +2342,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:G24">
-    <cfRule type="dataBar" priority="10">
+    <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2050,7 +2356,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H12">
-    <cfRule type="dataBar" priority="22">
+    <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2064,7 +2370,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:H24">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2078,7 +2384,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I12">
-    <cfRule type="dataBar" priority="21">
+    <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2092,7 +2398,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:I24">
-    <cfRule type="dataBar" priority="8">
+    <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2106,7 +2412,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J12">
-    <cfRule type="dataBar" priority="20">
+    <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2120,7 +2426,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:J24">
-    <cfRule type="dataBar" priority="7">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2134,7 +2440,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K12">
-    <cfRule type="dataBar" priority="19">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2148,7 +2454,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:K24">
-    <cfRule type="dataBar" priority="6">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2162,7 +2468,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L12">
-    <cfRule type="dataBar" priority="18">
+    <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2176,7 +2482,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15:L24">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2190,7 +2496,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M12">
-    <cfRule type="dataBar" priority="17">
+    <cfRule type="dataBar" priority="19">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2204,7 +2510,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M15:M24">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2218,7 +2524,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N12">
-    <cfRule type="dataBar" priority="16">
+    <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2232,7 +2538,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15:N24">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2246,7 +2552,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O12">
-    <cfRule type="dataBar" priority="15">
+    <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2260,7 +2566,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O15:O24">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2274,7 +2580,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P12">
-    <cfRule type="dataBar" priority="14">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2288,7 +2594,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P15:P24">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2302,8 +2608,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -2656,8 +2963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4354F9D2-63F6-4956-BC04-3299D7C8DB32}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30:K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -3426,7 +3733,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="dataBar" priority="16">
+    <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3440,7 +3747,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:D24">
-    <cfRule type="dataBar" priority="8">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3454,7 +3761,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="dataBar" priority="15">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3468,7 +3775,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:E24">
-    <cfRule type="dataBar" priority="7">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3482,7 +3789,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11">
-    <cfRule type="dataBar" priority="14">
+    <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3496,7 +3803,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:F24">
-    <cfRule type="dataBar" priority="6">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3510,7 +3817,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G11">
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3524,7 +3831,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:G24">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3538,7 +3845,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H11">
-    <cfRule type="dataBar" priority="12">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3552,7 +3859,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:H24">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3566,7 +3873,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="dataBar" priority="11">
+    <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3580,7 +3887,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:I24">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3594,7 +3901,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J11">
-    <cfRule type="dataBar" priority="10">
+    <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3608,7 +3915,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:J24">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3622,7 +3929,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3636,7 +3943,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:K24">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3868,4 +4175,1097 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3D9E08-D469-41E4-8D58-8A6B9704990D}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:Y25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:O13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="2" max="2" width="8.17578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.87890625" customWidth="1"/>
+    <col min="5" max="13" width="3.41015625" customWidth="1"/>
+    <col min="14" max="15" width="7.41015625" customWidth="1"/>
+    <col min="18" max="25" width="5.5859375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:25" x14ac:dyDescent="0.5">
+      <c r="B2" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="22"/>
+    </row>
+    <row r="3" spans="2:25" ht="34.35" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="16" t="str">
+        <f>js_tests!C14</f>
+        <v>Expected Rank</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="O3" s="18"/>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.5">
+      <c r="B4" s="13">
+        <f>js_tests!C2</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!D2,Table5[ssim (obartra)])</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!E2,Table5[ssim (darosh)])</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!F2,Table5[mse (jdf)],1)</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!H2,Table5[rmse (jdf)],1)</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!I2,Table5[nrmse (jdf)],1)</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!J2,Table5[inrmse (jdf)])</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!K2,Table5[nmse (jdf)],1)</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!L2,Table5[inmse (jdf)])</f>
+        <v>1</v>
+      </c>
+      <c r="L4" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!M2,Table5[mse (darosh)],1)</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="15">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!O2,Table5[msssim (darosh)])</f>
+        <v>1</v>
+      </c>
+      <c r="O4" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!P2,Table5[ssim (darosh msssim)])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.5">
+      <c r="B5" s="13">
+        <f>js_tests!C3</f>
+        <v>2</v>
+      </c>
+      <c r="C5" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!D3,Table5[ssim (obartra)])</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!E3,Table5[ssim (darosh)])</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!F3,Table5[mse (jdf)],1)</f>
+        <v>2</v>
+      </c>
+      <c r="F5" s="4">
+        <f>_xlfn.RANK.EQ(js_tests!G3,Table5[psnr (jdf)])+1</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!H3,Table5[rmse (jdf)],1)</f>
+        <v>2</v>
+      </c>
+      <c r="H5" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!I3,Table5[nrmse (jdf)],1)</f>
+        <v>2</v>
+      </c>
+      <c r="I5" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!J3,Table5[inrmse (jdf)])</f>
+        <v>2</v>
+      </c>
+      <c r="J5" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!K3,Table5[nmse (jdf)],1)</f>
+        <v>2</v>
+      </c>
+      <c r="K5" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!L3,Table5[inmse (jdf)])</f>
+        <v>2</v>
+      </c>
+      <c r="L5" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!M3,Table5[mse (darosh)],1)</f>
+        <v>2</v>
+      </c>
+      <c r="M5" s="6">
+        <f>_xlfn.RANK.EQ(js_tests!N3,Table5[psnr (darosh)])+1</f>
+        <v>2</v>
+      </c>
+      <c r="N5" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!O3,Table5[msssim (darosh)])</f>
+        <v>2</v>
+      </c>
+      <c r="O5" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!P3,Table5[ssim (darosh msssim)])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.5">
+      <c r="B6" s="13">
+        <f>js_tests!C4</f>
+        <v>3</v>
+      </c>
+      <c r="C6" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!D4,Table5[ssim (obartra)])</f>
+        <v>6</v>
+      </c>
+      <c r="D6" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!E4,Table5[ssim (darosh)])</f>
+        <v>6</v>
+      </c>
+      <c r="E6" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!F4,Table5[mse (jdf)],1)</f>
+        <v>3</v>
+      </c>
+      <c r="F6" s="4">
+        <f>_xlfn.RANK.EQ(js_tests!G4,Table5[psnr (jdf)])+1</f>
+        <v>3</v>
+      </c>
+      <c r="G6" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!H4,Table5[rmse (jdf)],1)</f>
+        <v>3</v>
+      </c>
+      <c r="H6" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!I4,Table5[nrmse (jdf)],1)</f>
+        <v>3</v>
+      </c>
+      <c r="I6" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!J4,Table5[inrmse (jdf)])</f>
+        <v>3</v>
+      </c>
+      <c r="J6" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!K4,Table5[nmse (jdf)],1)</f>
+        <v>3</v>
+      </c>
+      <c r="K6" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!L4,Table5[inmse (jdf)])</f>
+        <v>3</v>
+      </c>
+      <c r="L6" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!M4,Table5[mse (darosh)],1)</f>
+        <v>3</v>
+      </c>
+      <c r="M6" s="6">
+        <f>_xlfn.RANK.EQ(js_tests!N4,Table5[psnr (darosh)])+1</f>
+        <v>3</v>
+      </c>
+      <c r="N6" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!O4,Table5[msssim (darosh)])</f>
+        <v>4</v>
+      </c>
+      <c r="O6" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!P4,Table5[ssim (darosh msssim)])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.5">
+      <c r="B7" s="13">
+        <f>js_tests!C5</f>
+        <v>4</v>
+      </c>
+      <c r="C7" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!D5,Table5[ssim (obartra)])</f>
+        <v>7</v>
+      </c>
+      <c r="D7" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!E5,Table5[ssim (darosh)])</f>
+        <v>7</v>
+      </c>
+      <c r="E7" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!F5,Table5[mse (jdf)],1)</f>
+        <v>5</v>
+      </c>
+      <c r="F7" s="4">
+        <f>_xlfn.RANK.EQ(js_tests!G5,Table5[psnr (jdf)])+1</f>
+        <v>5</v>
+      </c>
+      <c r="G7" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!H5,Table5[rmse (jdf)],1)</f>
+        <v>5</v>
+      </c>
+      <c r="H7" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!I5,Table5[nrmse (jdf)],1)</f>
+        <v>5</v>
+      </c>
+      <c r="I7" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!J5,Table5[inrmse (jdf)])</f>
+        <v>5</v>
+      </c>
+      <c r="J7" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!K5,Table5[nmse (jdf)],1)</f>
+        <v>5</v>
+      </c>
+      <c r="K7" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!L5,Table5[inmse (jdf)])</f>
+        <v>5</v>
+      </c>
+      <c r="L7" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!M5,Table5[mse (darosh)],1)</f>
+        <v>5</v>
+      </c>
+      <c r="M7" s="6">
+        <f>_xlfn.RANK.EQ(js_tests!N5,Table5[psnr (darosh)])+1</f>
+        <v>5</v>
+      </c>
+      <c r="N7" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!O5,Table5[msssim (darosh)])</f>
+        <v>5</v>
+      </c>
+      <c r="O7" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!P5,Table5[ssim (darosh msssim)])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.5">
+      <c r="B8" s="13">
+        <f>js_tests!C6</f>
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!D6,Table5[ssim (obartra)])</f>
+        <v>8</v>
+      </c>
+      <c r="D8" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!E6,Table5[ssim (darosh)])</f>
+        <v>8</v>
+      </c>
+      <c r="E8" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!F6,Table5[mse (jdf)],1)</f>
+        <v>6</v>
+      </c>
+      <c r="F8" s="4">
+        <f>_xlfn.RANK.EQ(js_tests!G6,Table5[psnr (jdf)])+1</f>
+        <v>6</v>
+      </c>
+      <c r="G8" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!H6,Table5[rmse (jdf)],1)</f>
+        <v>6</v>
+      </c>
+      <c r="H8" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!I6,Table5[nrmse (jdf)],1)</f>
+        <v>6</v>
+      </c>
+      <c r="I8" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!J6,Table5[inrmse (jdf)])</f>
+        <v>6</v>
+      </c>
+      <c r="J8" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!K6,Table5[nmse (jdf)],1)</f>
+        <v>6</v>
+      </c>
+      <c r="K8" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!L6,Table5[inmse (jdf)])</f>
+        <v>6</v>
+      </c>
+      <c r="L8" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!M6,Table5[mse (darosh)],1)</f>
+        <v>6</v>
+      </c>
+      <c r="M8" s="6">
+        <f>_xlfn.RANK.EQ(js_tests!N6,Table5[psnr (darosh)])+1</f>
+        <v>6</v>
+      </c>
+      <c r="N8" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!O6,Table5[msssim (darosh)])</f>
+        <v>7</v>
+      </c>
+      <c r="O8" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!P6,Table5[ssim (darosh msssim)])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.5">
+      <c r="B9" s="13">
+        <f>js_tests!C7</f>
+        <v>6</v>
+      </c>
+      <c r="C9" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!D7,Table5[ssim (obartra)])</f>
+        <v>5</v>
+      </c>
+      <c r="D9" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!E7,Table5[ssim (darosh)])</f>
+        <v>5</v>
+      </c>
+      <c r="E9" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!F7,Table5[mse (jdf)],1)</f>
+        <v>4</v>
+      </c>
+      <c r="F9" s="4">
+        <f>_xlfn.RANK.EQ(js_tests!G7,Table5[psnr (jdf)])+1</f>
+        <v>4</v>
+      </c>
+      <c r="G9" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!H7,Table5[rmse (jdf)],1)</f>
+        <v>4</v>
+      </c>
+      <c r="H9" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!I7,Table5[nrmse (jdf)],1)</f>
+        <v>4</v>
+      </c>
+      <c r="I9" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!J7,Table5[inrmse (jdf)])</f>
+        <v>4</v>
+      </c>
+      <c r="J9" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!K7,Table5[nmse (jdf)],1)</f>
+        <v>4</v>
+      </c>
+      <c r="K9" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!L7,Table5[inmse (jdf)])</f>
+        <v>4</v>
+      </c>
+      <c r="L9" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!M7,Table5[mse (darosh)],1)</f>
+        <v>4</v>
+      </c>
+      <c r="M9" s="6">
+        <f>_xlfn.RANK.EQ(js_tests!N7,Table5[psnr (darosh)])+1</f>
+        <v>4</v>
+      </c>
+      <c r="N9" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!O7,Table5[msssim (darosh)])</f>
+        <v>3</v>
+      </c>
+      <c r="O9" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!P7,Table5[ssim (darosh msssim)])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.5">
+      <c r="B10" s="13">
+        <f>js_tests!C8</f>
+        <v>7</v>
+      </c>
+      <c r="C10" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!D8,Table5[ssim (obartra)])</f>
+        <v>3</v>
+      </c>
+      <c r="D10" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!E8,Table5[ssim (darosh)])</f>
+        <v>3</v>
+      </c>
+      <c r="E10" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!F8,Table5[mse (jdf)],1)</f>
+        <v>7</v>
+      </c>
+      <c r="F10" s="4">
+        <f>_xlfn.RANK.EQ(js_tests!G8,Table5[psnr (jdf)])+1</f>
+        <v>7</v>
+      </c>
+      <c r="G10" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!H8,Table5[rmse (jdf)],1)</f>
+        <v>7</v>
+      </c>
+      <c r="H10" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!I8,Table5[nrmse (jdf)],1)</f>
+        <v>7</v>
+      </c>
+      <c r="I10" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!J8,Table5[inrmse (jdf)])</f>
+        <v>7</v>
+      </c>
+      <c r="J10" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!K8,Table5[nmse (jdf)],1)</f>
+        <v>7</v>
+      </c>
+      <c r="K10" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!L8,Table5[inmse (jdf)])</f>
+        <v>7</v>
+      </c>
+      <c r="L10" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!M8,Table5[mse (darosh)],1)</f>
+        <v>7</v>
+      </c>
+      <c r="M10" s="6">
+        <f>_xlfn.RANK.EQ(js_tests!N8,Table5[psnr (darosh)])+1</f>
+        <v>7</v>
+      </c>
+      <c r="N10" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!O8,Table5[msssim (darosh)])</f>
+        <v>6</v>
+      </c>
+      <c r="O10" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!P8,Table5[ssim (darosh msssim)])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.5">
+      <c r="B11" s="13">
+        <f>js_tests!C9</f>
+        <v>8</v>
+      </c>
+      <c r="C11" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!D9,Table5[ssim (obartra)])</f>
+        <v>4</v>
+      </c>
+      <c r="D11" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!E9,Table5[ssim (darosh)])</f>
+        <v>4</v>
+      </c>
+      <c r="E11" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!F9,Table5[mse (jdf)],1)</f>
+        <v>9</v>
+      </c>
+      <c r="F11" s="4">
+        <f>_xlfn.RANK.EQ(js_tests!G9,Table5[psnr (jdf)])+1</f>
+        <v>9</v>
+      </c>
+      <c r="G11" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!H9,Table5[rmse (jdf)],1)</f>
+        <v>9</v>
+      </c>
+      <c r="H11" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!I9,Table5[nrmse (jdf)],1)</f>
+        <v>9</v>
+      </c>
+      <c r="I11" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!J9,Table5[inrmse (jdf)])</f>
+        <v>9</v>
+      </c>
+      <c r="J11" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!K9,Table5[nmse (jdf)],1)</f>
+        <v>9</v>
+      </c>
+      <c r="K11" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!L9,Table5[inmse (jdf)])</f>
+        <v>9</v>
+      </c>
+      <c r="L11" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!M9,Table5[mse (darosh)],1)</f>
+        <v>9</v>
+      </c>
+      <c r="M11" s="6">
+        <f>_xlfn.RANK.EQ(js_tests!N9,Table5[psnr (darosh)])+1</f>
+        <v>9</v>
+      </c>
+      <c r="N11" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!O9,Table5[msssim (darosh)])</f>
+        <v>8</v>
+      </c>
+      <c r="O11" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!P9,Table5[ssim (darosh msssim)])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.5">
+      <c r="B12" s="13">
+        <f>js_tests!C10</f>
+        <v>9</v>
+      </c>
+      <c r="C12" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!D10,Table5[ssim (obartra)])</f>
+        <v>9</v>
+      </c>
+      <c r="D12" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!E10,Table5[ssim (darosh)])</f>
+        <v>9</v>
+      </c>
+      <c r="E12" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!F10,Table5[mse (jdf)],1)</f>
+        <v>8</v>
+      </c>
+      <c r="F12" s="4">
+        <f>_xlfn.RANK.EQ(js_tests!G10,Table5[psnr (jdf)])+1</f>
+        <v>8</v>
+      </c>
+      <c r="G12" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!H10,Table5[rmse (jdf)],1)</f>
+        <v>8</v>
+      </c>
+      <c r="H12" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!I10,Table5[nrmse (jdf)],1)</f>
+        <v>8</v>
+      </c>
+      <c r="I12" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!J10,Table5[inrmse (jdf)])</f>
+        <v>8</v>
+      </c>
+      <c r="J12" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!K10,Table5[nmse (jdf)],1)</f>
+        <v>8</v>
+      </c>
+      <c r="K12" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!L10,Table5[inmse (jdf)])</f>
+        <v>8</v>
+      </c>
+      <c r="L12" s="5">
+        <f>_xlfn.RANK.EQ(js_tests!M10,Table5[mse (darosh)],1)</f>
+        <v>8</v>
+      </c>
+      <c r="M12" s="6">
+        <f>_xlfn.RANK.EQ(js_tests!N10,Table5[psnr (darosh)])+1</f>
+        <v>8</v>
+      </c>
+      <c r="N12" s="3">
+        <f>_xlfn.RANK.EQ(js_tests!O10,Table5[msssim (darosh)])</f>
+        <v>9</v>
+      </c>
+      <c r="O12" s="11">
+        <f>_xlfn.RANK.EQ(js_tests!P10,Table5[ssim (darosh msssim)])</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25" x14ac:dyDescent="0.5">
+      <c r="B13" s="14">
+        <f>js_tests!C11</f>
+        <v>10</v>
+      </c>
+      <c r="C13" s="7">
+        <f>_xlfn.RANK.EQ(js_tests!D11,Table5[ssim (obartra)])</f>
+        <v>10</v>
+      </c>
+      <c r="D13" s="12">
+        <f>_xlfn.RANK.EQ(js_tests!E11,Table5[ssim (darosh)])</f>
+        <v>10</v>
+      </c>
+      <c r="E13" s="7">
+        <f>_xlfn.RANK.EQ(js_tests!F11,Table5[mse (jdf)],1)</f>
+        <v>10</v>
+      </c>
+      <c r="F13" s="8">
+        <f>_xlfn.RANK.EQ(js_tests!G11,Table5[psnr (jdf)])+1</f>
+        <v>10</v>
+      </c>
+      <c r="G13" s="9">
+        <f>_xlfn.RANK.EQ(js_tests!H11,Table5[rmse (jdf)],1)</f>
+        <v>10</v>
+      </c>
+      <c r="H13" s="9">
+        <f>_xlfn.RANK.EQ(js_tests!I11,Table5[nrmse (jdf)],1)</f>
+        <v>10</v>
+      </c>
+      <c r="I13" s="9">
+        <f>_xlfn.RANK.EQ(js_tests!J11,Table5[inrmse (jdf)])</f>
+        <v>10</v>
+      </c>
+      <c r="J13" s="9">
+        <f>_xlfn.RANK.EQ(js_tests!K11,Table5[nmse (jdf)],1)</f>
+        <v>10</v>
+      </c>
+      <c r="K13" s="9">
+        <f>_xlfn.RANK.EQ(js_tests!L11,Table5[inmse (jdf)])</f>
+        <v>10</v>
+      </c>
+      <c r="L13" s="9">
+        <f>_xlfn.RANK.EQ(js_tests!M11,Table5[mse (darosh)],1)</f>
+        <v>10</v>
+      </c>
+      <c r="M13" s="10">
+        <f>_xlfn.RANK.EQ(js_tests!N11,Table5[psnr (darosh)])+1</f>
+        <v>10</v>
+      </c>
+      <c r="N13" s="7">
+        <f>_xlfn.RANK.EQ(js_tests!O11,Table5[msssim (darosh)])</f>
+        <v>10</v>
+      </c>
+      <c r="O13" s="12">
+        <f>_xlfn.RANK.EQ(js_tests!P11,Table5[ssim (darosh msssim)])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25" x14ac:dyDescent="0.5">
+      <c r="Q14" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="R14" s="27"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="23"/>
+      <c r="Y14" s="24"/>
+    </row>
+    <row r="15" spans="2:25" ht="32" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="Q15" s="25" t="str">
+        <f>Table6[[#Headers],[Expected rank]]</f>
+        <v>Expected rank</v>
+      </c>
+      <c r="R15" s="28" t="str">
+        <f>Table6[[#Headers],[mse]]</f>
+        <v>mse</v>
+      </c>
+      <c r="S15" s="31" t="str">
+        <f>Table6[[#Headers],[rmse]]</f>
+        <v>rmse</v>
+      </c>
+      <c r="T15" s="29" t="str">
+        <f>Table6[[#Headers],[psnr]]</f>
+        <v>psnr</v>
+      </c>
+      <c r="U15" s="30" t="str">
+        <f>Table6[[#Headers],[uqi]]</f>
+        <v>uqi</v>
+      </c>
+      <c r="V15" s="28" t="str">
+        <f>Table6[[#Headers],[ssim]]</f>
+        <v>ssim</v>
+      </c>
+      <c r="W15" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="X15" s="26" t="str">
+        <f>Table6[[#Headers],[scc]]</f>
+        <v>scc</v>
+      </c>
+      <c r="Y15" s="16" t="str">
+        <f>Table6[[#Headers],[vifp]]</f>
+        <v>vifp</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.5">
+      <c r="Q16" s="3">
+        <f>py_tests!C2</f>
+        <v>1</v>
+      </c>
+      <c r="R16" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!D2,Table6[mse],1)</f>
+        <v>1</v>
+      </c>
+      <c r="S16" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!E2,Table6[rmse],1)</f>
+        <v>1</v>
+      </c>
+      <c r="T16" s="15">
+        <v>1</v>
+      </c>
+      <c r="U16" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!G2,Table6[uqi],0)</f>
+        <v>1</v>
+      </c>
+      <c r="V16" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!H2,Table6[ssim],0)</f>
+        <v>1</v>
+      </c>
+      <c r="W16" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!I2,Table6[msssim],0)</f>
+        <v>1</v>
+      </c>
+      <c r="X16" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!J2,Table6[scc],0)</f>
+        <v>1</v>
+      </c>
+      <c r="Y16" s="13">
+        <f>_xlfn.RANK.EQ(py_tests!K2,Table6[vifp],0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="17:25" x14ac:dyDescent="0.5">
+      <c r="Q17" s="3">
+        <f>py_tests!C3</f>
+        <v>2</v>
+      </c>
+      <c r="R17" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!D3,Table6[mse],1)</f>
+        <v>2</v>
+      </c>
+      <c r="S17" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!E3,Table6[rmse],1)</f>
+        <v>2</v>
+      </c>
+      <c r="T17" s="6">
+        <f>_xlfn.RANK.EQ(py_tests!F3,Table6[psnr],0)+1</f>
+        <v>2</v>
+      </c>
+      <c r="U17" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!G3,Table6[uqi],0)</f>
+        <v>2</v>
+      </c>
+      <c r="V17" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!H3,Table6[ssim],0)</f>
+        <v>2</v>
+      </c>
+      <c r="W17" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!I3,Table6[msssim],0)</f>
+        <v>2</v>
+      </c>
+      <c r="X17" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!J3,Table6[scc],0)</f>
+        <v>2</v>
+      </c>
+      <c r="Y17" s="13">
+        <f>_xlfn.RANK.EQ(py_tests!K3,Table6[vifp],0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="17:25" x14ac:dyDescent="0.5">
+      <c r="Q18" s="3">
+        <f>py_tests!C4</f>
+        <v>3</v>
+      </c>
+      <c r="R18" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!D4,Table6[mse],1)</f>
+        <v>3</v>
+      </c>
+      <c r="S18" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!E4,Table6[rmse],1)</f>
+        <v>3</v>
+      </c>
+      <c r="T18" s="6">
+        <f>_xlfn.RANK.EQ(py_tests!F4,Table6[psnr],0)+1</f>
+        <v>3</v>
+      </c>
+      <c r="U18" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!G4,Table6[uqi],0)</f>
+        <v>3</v>
+      </c>
+      <c r="V18" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!H4,Table6[ssim],0)</f>
+        <v>6</v>
+      </c>
+      <c r="W18" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!I4,Table6[msssim],0)</f>
+        <v>5</v>
+      </c>
+      <c r="X18" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!J4,Table6[scc],0)</f>
+        <v>7</v>
+      </c>
+      <c r="Y18" s="13">
+        <f>_xlfn.RANK.EQ(py_tests!K4,Table6[vifp],0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="17:25" x14ac:dyDescent="0.5">
+      <c r="Q19" s="3">
+        <f>py_tests!C5</f>
+        <v>4</v>
+      </c>
+      <c r="R19" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!D5,Table6[mse],1)</f>
+        <v>5</v>
+      </c>
+      <c r="S19" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!E5,Table6[rmse],1)</f>
+        <v>5</v>
+      </c>
+      <c r="T19" s="6">
+        <f>_xlfn.RANK.EQ(py_tests!F5,Table6[psnr],0)+1</f>
+        <v>5</v>
+      </c>
+      <c r="U19" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!G5,Table6[uqi],0)</f>
+        <v>5</v>
+      </c>
+      <c r="V19" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!H5,Table6[ssim],0)</f>
+        <v>7</v>
+      </c>
+      <c r="W19" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!I5,Table6[msssim],0)</f>
+        <v>6</v>
+      </c>
+      <c r="X19" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!J5,Table6[scc],0)</f>
+        <v>10</v>
+      </c>
+      <c r="Y19" s="13">
+        <f>_xlfn.RANK.EQ(py_tests!K5,Table6[vifp],0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="17:25" x14ac:dyDescent="0.5">
+      <c r="Q20" s="3">
+        <f>py_tests!C6</f>
+        <v>5</v>
+      </c>
+      <c r="R20" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!D6,Table6[mse],1)</f>
+        <v>6</v>
+      </c>
+      <c r="S20" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!E6,Table6[rmse],1)</f>
+        <v>6</v>
+      </c>
+      <c r="T20" s="6">
+        <f>_xlfn.RANK.EQ(py_tests!F6,Table6[psnr],0)+1</f>
+        <v>6</v>
+      </c>
+      <c r="U20" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!G6,Table6[uqi],0)</f>
+        <v>6</v>
+      </c>
+      <c r="V20" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!H6,Table6[ssim],0)</f>
+        <v>8</v>
+      </c>
+      <c r="W20" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!I6,Table6[msssim],0)</f>
+        <v>8</v>
+      </c>
+      <c r="X20" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!J6,Table6[scc],0)</f>
+        <v>9</v>
+      </c>
+      <c r="Y20" s="13">
+        <f>_xlfn.RANK.EQ(py_tests!K6,Table6[vifp],0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="17:25" x14ac:dyDescent="0.5">
+      <c r="Q21" s="3">
+        <f>py_tests!C7</f>
+        <v>6</v>
+      </c>
+      <c r="R21" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!D7,Table6[mse],1)</f>
+        <v>4</v>
+      </c>
+      <c r="S21" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!E7,Table6[rmse],1)</f>
+        <v>4</v>
+      </c>
+      <c r="T21" s="6">
+        <f>_xlfn.RANK.EQ(py_tests!F7,Table6[psnr],0)+1</f>
+        <v>4</v>
+      </c>
+      <c r="U21" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!G7,Table6[uqi],0)</f>
+        <v>4</v>
+      </c>
+      <c r="V21" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!H7,Table6[ssim],0)</f>
+        <v>5</v>
+      </c>
+      <c r="W21" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!I7,Table6[msssim],0)</f>
+        <v>4</v>
+      </c>
+      <c r="X21" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!J7,Table6[scc],0)</f>
+        <v>6</v>
+      </c>
+      <c r="Y21" s="13">
+        <f>_xlfn.RANK.EQ(py_tests!K7,Table6[vifp],0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="17:25" x14ac:dyDescent="0.5">
+      <c r="Q22" s="3">
+        <f>py_tests!C8</f>
+        <v>7</v>
+      </c>
+      <c r="R22" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!D8,Table6[mse],1)</f>
+        <v>7</v>
+      </c>
+      <c r="S22" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!E8,Table6[rmse],1)</f>
+        <v>7</v>
+      </c>
+      <c r="T22" s="6">
+        <f>_xlfn.RANK.EQ(py_tests!F8,Table6[psnr],0)+1</f>
+        <v>7</v>
+      </c>
+      <c r="U22" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!G8,Table6[uqi],0)</f>
+        <v>7</v>
+      </c>
+      <c r="V22" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!H8,Table6[ssim],0)</f>
+        <v>4</v>
+      </c>
+      <c r="W22" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!I8,Table6[msssim],0)</f>
+        <v>3</v>
+      </c>
+      <c r="X22" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!J8,Table6[scc],0)</f>
+        <v>8</v>
+      </c>
+      <c r="Y22" s="13">
+        <f>_xlfn.RANK.EQ(py_tests!K8,Table6[vifp],0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="17:25" x14ac:dyDescent="0.5">
+      <c r="Q23" s="3">
+        <f>py_tests!C9</f>
+        <v>8</v>
+      </c>
+      <c r="R23" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!D9,Table6[mse],1)</f>
+        <v>9</v>
+      </c>
+      <c r="S23" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!E9,Table6[rmse],1)</f>
+        <v>9</v>
+      </c>
+      <c r="T23" s="6">
+        <f>_xlfn.RANK.EQ(py_tests!F9,Table6[psnr],0)+1</f>
+        <v>9</v>
+      </c>
+      <c r="U23" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!G9,Table6[uqi],0)</f>
+        <v>10</v>
+      </c>
+      <c r="V23" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!H9,Table6[ssim],0)</f>
+        <v>3</v>
+      </c>
+      <c r="W23" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!I9,Table6[msssim],0)</f>
+        <v>7</v>
+      </c>
+      <c r="X23" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!J9,Table6[scc],0)</f>
+        <v>5</v>
+      </c>
+      <c r="Y23" s="13">
+        <f>_xlfn.RANK.EQ(py_tests!K9,Table6[vifp],0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="17:25" x14ac:dyDescent="0.5">
+      <c r="Q24" s="3">
+        <f>py_tests!C10</f>
+        <v>9</v>
+      </c>
+      <c r="R24" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!D10,Table6[mse],1)</f>
+        <v>8</v>
+      </c>
+      <c r="S24" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!E10,Table6[rmse],1)</f>
+        <v>8</v>
+      </c>
+      <c r="T24" s="6">
+        <f>_xlfn.RANK.EQ(py_tests!F10,Table6[psnr],0)+1</f>
+        <v>8</v>
+      </c>
+      <c r="U24" s="5">
+        <f>_xlfn.RANK.EQ(py_tests!G10,Table6[uqi],0)</f>
+        <v>8</v>
+      </c>
+      <c r="V24" s="3">
+        <f>_xlfn.RANK.EQ(py_tests!H10,Table6[ssim],0)</f>
+        <v>9</v>
+      </c>
+      <c r="W24" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!I10,Table6[msssim],0)</f>
+        <v>9</v>
+      </c>
+      <c r="X24" s="11">
+        <f>_xlfn.RANK.EQ(py_tests!J10,Table6[scc],0)</f>
+        <v>4</v>
+      </c>
+      <c r="Y24" s="13">
+        <f>_xlfn.RANK.EQ(py_tests!K10,Table6[vifp],0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="17:25" x14ac:dyDescent="0.5">
+      <c r="Q25" s="7">
+        <f>py_tests!C11</f>
+        <v>10</v>
+      </c>
+      <c r="R25" s="7">
+        <f>_xlfn.RANK.EQ(py_tests!D11,Table6[mse],1)</f>
+        <v>10</v>
+      </c>
+      <c r="S25" s="9">
+        <f>_xlfn.RANK.EQ(py_tests!E11,Table6[rmse],1)</f>
+        <v>10</v>
+      </c>
+      <c r="T25" s="10">
+        <f>_xlfn.RANK.EQ(py_tests!F11,Table6[psnr],0)+1</f>
+        <v>10</v>
+      </c>
+      <c r="U25" s="9">
+        <f>_xlfn.RANK.EQ(py_tests!G11,Table6[uqi],0)</f>
+        <v>9</v>
+      </c>
+      <c r="V25" s="7">
+        <f>_xlfn.RANK.EQ(py_tests!H11,Table6[ssim],0)</f>
+        <v>10</v>
+      </c>
+      <c r="W25" s="12">
+        <f>_xlfn.RANK.EQ(py_tests!I11,Table6[msssim],0)</f>
+        <v>10</v>
+      </c>
+      <c r="X25" s="12">
+        <f>_xlfn.RANK.EQ(py_tests!J11,Table6[scc],0)</f>
+        <v>3</v>
+      </c>
+      <c r="Y25" s="14">
+        <f>_xlfn.RANK.EQ(py_tests!K11,Table6[vifp],0)</f>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="Q14:Y14"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C4:O13">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>$B4&lt;&gt;C4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R16:Y25">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>$Q16&lt;&gt;R16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="86" orientation="landscape" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
vnvreport: fix lib refs, added graphs
</commit_message>
<xml_diff>
--- a/docs/VnVReport/test-analysis/metric_results_analysis.xlsx
+++ b/docs/VnVReport/test-analysis/metric_results_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joedf\Documents\GitHub\CAS741_w23\docs\VnVReport\test-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EF94F2-8ADB-4A75-A8E5-6DC126E915F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7196445-34B3-41F8-B96D-407BDCED247E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15733" activeTab="2" xr2:uid="{5B20B560-2675-4915-B90A-97D8720C64BF}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15733" xr2:uid="{5B20B560-2675-4915-B90A-97D8720C64BF}"/>
   </bookViews>
   <sheets>
     <sheet name="js_tests" sheetId="1" r:id="rId1"/>
@@ -467,15 +467,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -500,6 +499,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -509,73 +526,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <fill>
         <patternFill>
@@ -666,6 +630,2956 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Normalized Image Metrics vs Expected Rank (js-tests)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>js_tests!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ssim (obartra)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>js_tests!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99473024061113002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.62188645691851496</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.60480462305112603</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.58690539318117196</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.63211237763649597</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.66117361179510803</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65705322854326897</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.42572597556185399</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.37342345065857002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-C08C-4E15-8739-565CB621F6A0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>js_tests!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ssim (darosh)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>js_tests!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99502961066274898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.63140357299275196</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61446688859287502</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59699511382759396</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.64183300224769602</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.67204597697259205</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.66671584165123399</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.43889027386031199</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.38487461805746098</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-C08C-4E15-8739-565CB621F6A0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>js_tests!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>inrmse (jdf)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>js_tests!$J$2:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99553801998356595</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.867783366567346</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.86736353196006899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86604340595247997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.86746077951937495</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.86038100335856105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.82859725965531394</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.83655986721563402</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.82080813838561695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-C08C-4E15-8739-565CB621F6A0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>js_tests!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>inmse (jdf)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>js_tests!$L$2:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99998009073433203</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98251876184373499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98240756734589196</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98205563091118797</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.982433355034388</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.980506535776838</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97062110060233198</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.97328732299542897</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.96789027673117101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-C08C-4E15-8739-565CB621F6A0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>js_tests!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>msssim (darosh)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>js_tests!$O$2:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99564114922920399</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69525111251523397</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.69037216313553396</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.67536907253123502</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.70172255802651295</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.68720842669072102</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.58596217366492098</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.46978076549597497</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.30769984815057599</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-C08C-4E15-8739-565CB621F6A0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>js_tests!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ssim (darosh msssim)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>js_tests!$P$2:$P$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99502961066274898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.63140357299275196</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61446688859287502</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59699511382759396</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.64183300224769602</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.67204597697259205</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.66671584165123399</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.43889027386031199</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.38487461805746098</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-C08C-4E15-8739-565CB621F6A0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="65358191"/>
+        <c:axId val="115991807"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="65358191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Expected Rank Order</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="115991807"/>
+        <c:crossesAt val="-0.1"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="115991807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.30000000000000004"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Metric value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="65358191"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Normalized Image Metrics vs Expected Rank (py-tests)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>py_tests!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>uqi</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>py_tests!$G$2:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99990386372957896</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89511269174578101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89419083054185</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.89248771148239503</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89494822886650205</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.88521415561180805</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.84594496194603297</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.86603415043491205</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.84990145368064396</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-2491-4BFF-8C24-A626810A272B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>py_tests!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ssim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>py_tests!$H$2:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99478566549507097</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.596365728814643</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.57927040378633798</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56237452048764702</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.60691767837225596</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.64018453456645796</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.651588220399267</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.43748814092141097</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.41091198980025301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-2491-4BFF-8C24-A626810A272B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>py_tests!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>msssim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>py_tests!$I$2:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99854740875854098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.74866981771580998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.73601952339450505</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.72139583934346496</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75529128617046604</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.76675555472539803</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.72334291405308204</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.52012577158205098</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.39492782785722702</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-2491-4BFF-8C24-A626810A272B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>py_tests!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>scc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>py_tests!$J$2:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.41610000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.41579442276733802</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.5979277352877301E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-9.2502997954640499E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-8.6387236014050196E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.8400392430435099E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.6701337618850399E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.9943854617496896E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5698465859403201E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8177408242078001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-2491-4BFF-8C24-A626810A272B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>py_tests!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>vifp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>py_tests!$K$2:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.999999999987773</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99940217861168801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2888779528166905E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.04887663710812E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.7928354080974603E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3848110126864893E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.3947721626114104E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.6376578035637302E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1264937837956898E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0912003884400399E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-2491-4BFF-8C24-A626810A272B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="65358191"/>
+        <c:axId val="115991807"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="65358191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Expected Rank Order</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="115991807"/>
+        <c:crossesAt val="-0.1"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="115991807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Metric value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="65358191"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>326688</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>173980</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>223188</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>133313</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3FD7264-615E-4BAE-827C-AA6407915BBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>586314</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>25397</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>478580</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>166764</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7D77539-FF46-7A13-3C76-D7950E46FBBE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{743264BA-2DDD-4564-9814-49BBFF2CEDA7}" name="Table5" displayName="Table5" ref="A1:P11" totalsRowShown="0">
   <autoFilter ref="A1:P11" xr:uid="{743264BA-2DDD-4564-9814-49BBFF2CEDA7}"/>
@@ -676,19 +3590,19 @@
     <tableColumn id="1" xr3:uid="{9611E537-4FE5-4C2D-9563-28B4D98E46B1}" name="#"/>
     <tableColumn id="2" xr3:uid="{F4267E20-0B79-4BB1-9ED6-D1F2798542E5}" name="testname"/>
     <tableColumn id="3" xr3:uid="{667F5C2D-228D-46C1-BF1E-AB83553AA98F}" name="Expected Rank"/>
-    <tableColumn id="4" xr3:uid="{A9B1C654-46D5-4D47-A59D-62A25EA835D9}" name="ssim (obartra)" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{27447F7F-34C1-450D-B649-BCD291EC9D27}" name="ssim (darosh)" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{BA47D22F-0BBA-4283-ADCA-CC3CFE1E00CC}" name="mse (jdf)" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{9B189C05-7059-4C40-B98C-AE4D4F0028F6}" name="psnr (jdf)" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{3B3AD642-EF8B-4A91-AE92-473ADB0DB518}" name="rmse (jdf)" dataDxfId="23"/>
-    <tableColumn id="9" xr3:uid="{B3BD767A-29A9-4F0D-B199-284EA05BA820}" name="nrmse (jdf)" dataDxfId="22"/>
-    <tableColumn id="10" xr3:uid="{E411ECA4-67A6-4CDA-9DC6-62CC7BCB1ED7}" name="inrmse (jdf)" dataDxfId="21"/>
-    <tableColumn id="11" xr3:uid="{A3FF7C39-6883-4E46-B55D-AC2F71D6EACF}" name="nmse (jdf)" dataDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{E1B8E126-AA92-44F1-8714-BB56F7585F25}" name="inmse (jdf)" dataDxfId="19"/>
-    <tableColumn id="13" xr3:uid="{C6C61EA8-C8B6-4697-9BE2-F7E000E16A25}" name="mse (darosh)" dataDxfId="18"/>
-    <tableColumn id="14" xr3:uid="{9E237621-BCB6-4CD4-81F6-A4086220EAF0}" name="psnr (darosh)" dataDxfId="17"/>
-    <tableColumn id="15" xr3:uid="{926C9206-BF6F-428E-9487-F8F4288AA3D0}" name="msssim (darosh)" dataDxfId="16"/>
-    <tableColumn id="16" xr3:uid="{7BC4D969-0313-4FC7-9DDF-FAB4C8AB41AD}" name="ssim (darosh msssim)" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{A9B1C654-46D5-4D47-A59D-62A25EA835D9}" name="ssim (obartra)" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{27447F7F-34C1-450D-B649-BCD291EC9D27}" name="ssim (darosh)" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{BA47D22F-0BBA-4283-ADCA-CC3CFE1E00CC}" name="mse (jdf)" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{9B189C05-7059-4C40-B98C-AE4D4F0028F6}" name="psnr (jdf)" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{3B3AD642-EF8B-4A91-AE92-473ADB0DB518}" name="rmse (jdf)" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{B3BD767A-29A9-4F0D-B199-284EA05BA820}" name="nrmse (jdf)" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{E411ECA4-67A6-4CDA-9DC6-62CC7BCB1ED7}" name="inrmse (jdf)" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{A3FF7C39-6883-4E46-B55D-AC2F71D6EACF}" name="nmse (jdf)" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{E1B8E126-AA92-44F1-8714-BB56F7585F25}" name="inmse (jdf)" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{C6C61EA8-C8B6-4697-9BE2-F7E000E16A25}" name="mse (darosh)" dataDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{9E237621-BCB6-4CD4-81F6-A4086220EAF0}" name="psnr (darosh)" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{926C9206-BF6F-428E-9487-F8F4288AA3D0}" name="msssim (darosh)" dataDxfId="11"/>
+    <tableColumn id="16" xr3:uid="{7BC4D969-0313-4FC7-9DDF-FAB4C8AB41AD}" name="ssim (darosh msssim)" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -704,14 +3618,14 @@
     <tableColumn id="1" xr3:uid="{F7FE2A69-0D8E-49C4-80D3-BF8C23D0A027}" name="#"/>
     <tableColumn id="2" xr3:uid="{E2042B5B-9F31-463B-B5E0-4E2BBE1367F2}" name="testname"/>
     <tableColumn id="3" xr3:uid="{A3B370FA-A8E4-46C6-9439-A63E81737EFA}" name="Expected rank"/>
-    <tableColumn id="4" xr3:uid="{48C3E892-DFED-4EE2-A0D8-6306DCA34237}" name="mse" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{7CE22FCF-DC21-4054-8A35-B2C1101FA1C8}" name="rmse" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{5AE8EBCB-89A9-4705-A221-32289F3AFAEC}" name="psnr" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{861346B0-7E61-45D5-9D7E-1D21897B881E}" name="uqi" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{F5BCC34F-D45E-4B6D-BC5A-31FC723553B1}" name="ssim" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{4FB8FA19-043E-49A7-9018-53C3A3D83C08}" name="msssim" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{511E004F-6D7D-4886-BD9F-7CDCD82D3998}" name="scc" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{2C7229B4-3D0C-489A-BD8D-4436AC33D976}" name="vifp" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{48C3E892-DFED-4EE2-A0D8-6306DCA34237}" name="mse" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{7CE22FCF-DC21-4054-8A35-B2C1101FA1C8}" name="rmse" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{5AE8EBCB-89A9-4705-A221-32289F3AFAEC}" name="psnr" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{861346B0-7E61-45D5-9D7E-1D21897B881E}" name="uqi" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{F5BCC34F-D45E-4B6D-BC5A-31FC723553B1}" name="ssim" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{4FB8FA19-043E-49A7-9018-53C3A3D83C08}" name="msssim" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{511E004F-6D7D-4886-BD9F-7CDCD82D3998}" name="scc" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{2C7229B4-3D0C-489A-BD8D-4436AC33D976}" name="vifp" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1016,8 +3930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B92C74-347A-4EDB-A0CE-4F0C99A5E60F}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2609,8 +5523,9 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -2963,8 +5878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4354F9D2-63F6-4956-BC04-3299D7C8DB32}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:K40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -3957,8 +6872,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -4184,7 +7100,7 @@
   </sheetPr>
   <dimension ref="B2:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:O13"/>
     </sheetView>
   </sheetViews>
@@ -4198,50 +7114,50 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:25" x14ac:dyDescent="0.5">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="22"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="27"/>
     </row>
     <row r="3" spans="2:25" ht="34.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="16" t="str">
+      <c r="B3" s="15" t="str">
         <f>js_tests!C14</f>
         <v>Expected Rank</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="17" t="s">
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="O3" s="18"/>
+      <c r="O3" s="24"/>
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.5">
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <f>js_tests!C2</f>
         <v>1</v>
       </c>
@@ -4249,7 +7165,7 @@
         <f>_xlfn.RANK.EQ(js_tests!D2,Table5[ssim (obartra)])</f>
         <v>1</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <f>_xlfn.RANK.EQ(js_tests!E2,Table5[ssim (darosh)])</f>
         <v>1</v>
       </c>
@@ -4257,47 +7173,47 @@
         <f>_xlfn.RANK.EQ(js_tests!F2,Table5[mse (jdf)],1)</f>
         <v>1</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4">
         <f>_xlfn.RANK.EQ(js_tests!H2,Table5[rmse (jdf)],1)</f>
         <v>1</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4">
         <f>_xlfn.RANK.EQ(js_tests!I2,Table5[nrmse (jdf)],1)</f>
         <v>1</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4">
         <f>_xlfn.RANK.EQ(js_tests!J2,Table5[inrmse (jdf)])</f>
         <v>1</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4">
         <f>_xlfn.RANK.EQ(js_tests!K2,Table5[nmse (jdf)],1)</f>
         <v>1</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4">
         <f>_xlfn.RANK.EQ(js_tests!L2,Table5[inmse (jdf)])</f>
         <v>1</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4">
         <f>_xlfn.RANK.EQ(js_tests!M2,Table5[mse (darosh)],1)</f>
         <v>1</v>
       </c>
-      <c r="M4" s="15">
+      <c r="M4" s="14">
         <v>1</v>
       </c>
       <c r="N4" s="3">
         <f>_xlfn.RANK.EQ(js_tests!O2,Table5[msssim (darosh)])</f>
         <v>1</v>
       </c>
-      <c r="O4" s="11">
+      <c r="O4" s="10">
         <f>_xlfn.RANK.EQ(js_tests!P2,Table5[ssim (darosh msssim)])</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.5">
-      <c r="B5" s="13">
+      <c r="B5" s="12">
         <f>js_tests!C3</f>
         <v>2</v>
       </c>
@@ -4305,7 +7221,7 @@
         <f>_xlfn.RANK.EQ(js_tests!D3,Table5[ssim (obartra)])</f>
         <v>2</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <f>_xlfn.RANK.EQ(js_tests!E3,Table5[ssim (darosh)])</f>
         <v>2</v>
       </c>
@@ -4317,31 +7233,31 @@
         <f>_xlfn.RANK.EQ(js_tests!G3,Table5[psnr (jdf)])+1</f>
         <v>2</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5">
         <f>_xlfn.RANK.EQ(js_tests!H3,Table5[rmse (jdf)],1)</f>
         <v>2</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5">
         <f>_xlfn.RANK.EQ(js_tests!I3,Table5[nrmse (jdf)],1)</f>
         <v>2</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5">
         <f>_xlfn.RANK.EQ(js_tests!J3,Table5[inrmse (jdf)])</f>
         <v>2</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5">
         <f>_xlfn.RANK.EQ(js_tests!K3,Table5[nmse (jdf)],1)</f>
         <v>2</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5">
         <f>_xlfn.RANK.EQ(js_tests!L3,Table5[inmse (jdf)])</f>
         <v>2</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5">
         <f>_xlfn.RANK.EQ(js_tests!M3,Table5[mse (darosh)],1)</f>
         <v>2</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="5">
         <f>_xlfn.RANK.EQ(js_tests!N3,Table5[psnr (darosh)])+1</f>
         <v>2</v>
       </c>
@@ -4349,13 +7265,13 @@
         <f>_xlfn.RANK.EQ(js_tests!O3,Table5[msssim (darosh)])</f>
         <v>2</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="10">
         <f>_xlfn.RANK.EQ(js_tests!P3,Table5[ssim (darosh msssim)])</f>
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.5">
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <f>js_tests!C4</f>
         <v>3</v>
       </c>
@@ -4363,7 +7279,7 @@
         <f>_xlfn.RANK.EQ(js_tests!D4,Table5[ssim (obartra)])</f>
         <v>6</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <f>_xlfn.RANK.EQ(js_tests!E4,Table5[ssim (darosh)])</f>
         <v>6</v>
       </c>
@@ -4375,31 +7291,31 @@
         <f>_xlfn.RANK.EQ(js_tests!G4,Table5[psnr (jdf)])+1</f>
         <v>3</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6">
         <f>_xlfn.RANK.EQ(js_tests!H4,Table5[rmse (jdf)],1)</f>
         <v>3</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6">
         <f>_xlfn.RANK.EQ(js_tests!I4,Table5[nrmse (jdf)],1)</f>
         <v>3</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6">
         <f>_xlfn.RANK.EQ(js_tests!J4,Table5[inrmse (jdf)])</f>
         <v>3</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6">
         <f>_xlfn.RANK.EQ(js_tests!K4,Table5[nmse (jdf)],1)</f>
         <v>3</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6">
         <f>_xlfn.RANK.EQ(js_tests!L4,Table5[inmse (jdf)])</f>
         <v>3</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6">
         <f>_xlfn.RANK.EQ(js_tests!M4,Table5[mse (darosh)],1)</f>
         <v>3</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="5">
         <f>_xlfn.RANK.EQ(js_tests!N4,Table5[psnr (darosh)])+1</f>
         <v>3</v>
       </c>
@@ -4407,13 +7323,13 @@
         <f>_xlfn.RANK.EQ(js_tests!O4,Table5[msssim (darosh)])</f>
         <v>4</v>
       </c>
-      <c r="O6" s="11">
+      <c r="O6" s="10">
         <f>_xlfn.RANK.EQ(js_tests!P4,Table5[ssim (darosh msssim)])</f>
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.5">
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <f>js_tests!C5</f>
         <v>4</v>
       </c>
@@ -4421,7 +7337,7 @@
         <f>_xlfn.RANK.EQ(js_tests!D5,Table5[ssim (obartra)])</f>
         <v>7</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <f>_xlfn.RANK.EQ(js_tests!E5,Table5[ssim (darosh)])</f>
         <v>7</v>
       </c>
@@ -4433,31 +7349,31 @@
         <f>_xlfn.RANK.EQ(js_tests!G5,Table5[psnr (jdf)])+1</f>
         <v>5</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7">
         <f>_xlfn.RANK.EQ(js_tests!H5,Table5[rmse (jdf)],1)</f>
         <v>5</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7">
         <f>_xlfn.RANK.EQ(js_tests!I5,Table5[nrmse (jdf)],1)</f>
         <v>5</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7">
         <f>_xlfn.RANK.EQ(js_tests!J5,Table5[inrmse (jdf)])</f>
         <v>5</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7">
         <f>_xlfn.RANK.EQ(js_tests!K5,Table5[nmse (jdf)],1)</f>
         <v>5</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7">
         <f>_xlfn.RANK.EQ(js_tests!L5,Table5[inmse (jdf)])</f>
         <v>5</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7">
         <f>_xlfn.RANK.EQ(js_tests!M5,Table5[mse (darosh)],1)</f>
         <v>5</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="5">
         <f>_xlfn.RANK.EQ(js_tests!N5,Table5[psnr (darosh)])+1</f>
         <v>5</v>
       </c>
@@ -4465,13 +7381,13 @@
         <f>_xlfn.RANK.EQ(js_tests!O5,Table5[msssim (darosh)])</f>
         <v>5</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="10">
         <f>_xlfn.RANK.EQ(js_tests!P5,Table5[ssim (darosh msssim)])</f>
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.5">
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <f>js_tests!C6</f>
         <v>5</v>
       </c>
@@ -4479,7 +7395,7 @@
         <f>_xlfn.RANK.EQ(js_tests!D6,Table5[ssim (obartra)])</f>
         <v>8</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <f>_xlfn.RANK.EQ(js_tests!E6,Table5[ssim (darosh)])</f>
         <v>8</v>
       </c>
@@ -4491,31 +7407,31 @@
         <f>_xlfn.RANK.EQ(js_tests!G6,Table5[psnr (jdf)])+1</f>
         <v>6</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8">
         <f>_xlfn.RANK.EQ(js_tests!H6,Table5[rmse (jdf)],1)</f>
         <v>6</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8">
         <f>_xlfn.RANK.EQ(js_tests!I6,Table5[nrmse (jdf)],1)</f>
         <v>6</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8">
         <f>_xlfn.RANK.EQ(js_tests!J6,Table5[inrmse (jdf)])</f>
         <v>6</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8">
         <f>_xlfn.RANK.EQ(js_tests!K6,Table5[nmse (jdf)],1)</f>
         <v>6</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8">
         <f>_xlfn.RANK.EQ(js_tests!L6,Table5[inmse (jdf)])</f>
         <v>6</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8">
         <f>_xlfn.RANK.EQ(js_tests!M6,Table5[mse (darosh)],1)</f>
         <v>6</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="5">
         <f>_xlfn.RANK.EQ(js_tests!N6,Table5[psnr (darosh)])+1</f>
         <v>6</v>
       </c>
@@ -4523,13 +7439,13 @@
         <f>_xlfn.RANK.EQ(js_tests!O6,Table5[msssim (darosh)])</f>
         <v>7</v>
       </c>
-      <c r="O8" s="11">
+      <c r="O8" s="10">
         <f>_xlfn.RANK.EQ(js_tests!P6,Table5[ssim (darosh msssim)])</f>
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.5">
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <f>js_tests!C7</f>
         <v>6</v>
       </c>
@@ -4537,7 +7453,7 @@
         <f>_xlfn.RANK.EQ(js_tests!D7,Table5[ssim (obartra)])</f>
         <v>5</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <f>_xlfn.RANK.EQ(js_tests!E7,Table5[ssim (darosh)])</f>
         <v>5</v>
       </c>
@@ -4549,31 +7465,31 @@
         <f>_xlfn.RANK.EQ(js_tests!G7,Table5[psnr (jdf)])+1</f>
         <v>4</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9">
         <f>_xlfn.RANK.EQ(js_tests!H7,Table5[rmse (jdf)],1)</f>
         <v>4</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9">
         <f>_xlfn.RANK.EQ(js_tests!I7,Table5[nrmse (jdf)],1)</f>
         <v>4</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9">
         <f>_xlfn.RANK.EQ(js_tests!J7,Table5[inrmse (jdf)])</f>
         <v>4</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9">
         <f>_xlfn.RANK.EQ(js_tests!K7,Table5[nmse (jdf)],1)</f>
         <v>4</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9">
         <f>_xlfn.RANK.EQ(js_tests!L7,Table5[inmse (jdf)])</f>
         <v>4</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9">
         <f>_xlfn.RANK.EQ(js_tests!M7,Table5[mse (darosh)],1)</f>
         <v>4</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="5">
         <f>_xlfn.RANK.EQ(js_tests!N7,Table5[psnr (darosh)])+1</f>
         <v>4</v>
       </c>
@@ -4581,13 +7497,13 @@
         <f>_xlfn.RANK.EQ(js_tests!O7,Table5[msssim (darosh)])</f>
         <v>3</v>
       </c>
-      <c r="O9" s="11">
+      <c r="O9" s="10">
         <f>_xlfn.RANK.EQ(js_tests!P7,Table5[ssim (darosh msssim)])</f>
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.5">
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <f>js_tests!C8</f>
         <v>7</v>
       </c>
@@ -4595,7 +7511,7 @@
         <f>_xlfn.RANK.EQ(js_tests!D8,Table5[ssim (obartra)])</f>
         <v>3</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <f>_xlfn.RANK.EQ(js_tests!E8,Table5[ssim (darosh)])</f>
         <v>3</v>
       </c>
@@ -4607,31 +7523,31 @@
         <f>_xlfn.RANK.EQ(js_tests!G8,Table5[psnr (jdf)])+1</f>
         <v>7</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10">
         <f>_xlfn.RANK.EQ(js_tests!H8,Table5[rmse (jdf)],1)</f>
         <v>7</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10">
         <f>_xlfn.RANK.EQ(js_tests!I8,Table5[nrmse (jdf)],1)</f>
         <v>7</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10">
         <f>_xlfn.RANK.EQ(js_tests!J8,Table5[inrmse (jdf)])</f>
         <v>7</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10">
         <f>_xlfn.RANK.EQ(js_tests!K8,Table5[nmse (jdf)],1)</f>
         <v>7</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10">
         <f>_xlfn.RANK.EQ(js_tests!L8,Table5[inmse (jdf)])</f>
         <v>7</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10">
         <f>_xlfn.RANK.EQ(js_tests!M8,Table5[mse (darosh)],1)</f>
         <v>7</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="5">
         <f>_xlfn.RANK.EQ(js_tests!N8,Table5[psnr (darosh)])+1</f>
         <v>7</v>
       </c>
@@ -4639,13 +7555,13 @@
         <f>_xlfn.RANK.EQ(js_tests!O8,Table5[msssim (darosh)])</f>
         <v>6</v>
       </c>
-      <c r="O10" s="11">
+      <c r="O10" s="10">
         <f>_xlfn.RANK.EQ(js_tests!P8,Table5[ssim (darosh msssim)])</f>
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.5">
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <f>js_tests!C9</f>
         <v>8</v>
       </c>
@@ -4653,7 +7569,7 @@
         <f>_xlfn.RANK.EQ(js_tests!D9,Table5[ssim (obartra)])</f>
         <v>4</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <f>_xlfn.RANK.EQ(js_tests!E9,Table5[ssim (darosh)])</f>
         <v>4</v>
       </c>
@@ -4665,31 +7581,31 @@
         <f>_xlfn.RANK.EQ(js_tests!G9,Table5[psnr (jdf)])+1</f>
         <v>9</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11">
         <f>_xlfn.RANK.EQ(js_tests!H9,Table5[rmse (jdf)],1)</f>
         <v>9</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11">
         <f>_xlfn.RANK.EQ(js_tests!I9,Table5[nrmse (jdf)],1)</f>
         <v>9</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11">
         <f>_xlfn.RANK.EQ(js_tests!J9,Table5[inrmse (jdf)])</f>
         <v>9</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11">
         <f>_xlfn.RANK.EQ(js_tests!K9,Table5[nmse (jdf)],1)</f>
         <v>9</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11">
         <f>_xlfn.RANK.EQ(js_tests!L9,Table5[inmse (jdf)])</f>
         <v>9</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11">
         <f>_xlfn.RANK.EQ(js_tests!M9,Table5[mse (darosh)],1)</f>
         <v>9</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="5">
         <f>_xlfn.RANK.EQ(js_tests!N9,Table5[psnr (darosh)])+1</f>
         <v>9</v>
       </c>
@@ -4697,13 +7613,13 @@
         <f>_xlfn.RANK.EQ(js_tests!O9,Table5[msssim (darosh)])</f>
         <v>8</v>
       </c>
-      <c r="O11" s="11">
+      <c r="O11" s="10">
         <f>_xlfn.RANK.EQ(js_tests!P9,Table5[ssim (darosh msssim)])</f>
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.5">
-      <c r="B12" s="13">
+      <c r="B12" s="12">
         <f>js_tests!C10</f>
         <v>9</v>
       </c>
@@ -4711,7 +7627,7 @@
         <f>_xlfn.RANK.EQ(js_tests!D10,Table5[ssim (obartra)])</f>
         <v>9</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <f>_xlfn.RANK.EQ(js_tests!E10,Table5[ssim (darosh)])</f>
         <v>9</v>
       </c>
@@ -4723,31 +7639,31 @@
         <f>_xlfn.RANK.EQ(js_tests!G10,Table5[psnr (jdf)])+1</f>
         <v>8</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12">
         <f>_xlfn.RANK.EQ(js_tests!H10,Table5[rmse (jdf)],1)</f>
         <v>8</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12">
         <f>_xlfn.RANK.EQ(js_tests!I10,Table5[nrmse (jdf)],1)</f>
         <v>8</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12">
         <f>_xlfn.RANK.EQ(js_tests!J10,Table5[inrmse (jdf)])</f>
         <v>8</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12">
         <f>_xlfn.RANK.EQ(js_tests!K10,Table5[nmse (jdf)],1)</f>
         <v>8</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12">
         <f>_xlfn.RANK.EQ(js_tests!L10,Table5[inmse (jdf)])</f>
         <v>8</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12">
         <f>_xlfn.RANK.EQ(js_tests!M10,Table5[mse (darosh)],1)</f>
         <v>8</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="5">
         <f>_xlfn.RANK.EQ(js_tests!N10,Table5[psnr (darosh)])+1</f>
         <v>8</v>
       </c>
@@ -4755,115 +7671,115 @@
         <f>_xlfn.RANK.EQ(js_tests!O10,Table5[msssim (darosh)])</f>
         <v>9</v>
       </c>
-      <c r="O12" s="11">
+      <c r="O12" s="10">
         <f>_xlfn.RANK.EQ(js_tests!P10,Table5[ssim (darosh msssim)])</f>
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.5">
-      <c r="B13" s="14">
+      <c r="B13" s="13">
         <f>js_tests!C11</f>
         <v>10</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <f>_xlfn.RANK.EQ(js_tests!D11,Table5[ssim (obartra)])</f>
         <v>10</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="11">
         <f>_xlfn.RANK.EQ(js_tests!E11,Table5[ssim (darosh)])</f>
         <v>10</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <f>_xlfn.RANK.EQ(js_tests!F11,Table5[mse (jdf)],1)</f>
         <v>10</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <f>_xlfn.RANK.EQ(js_tests!G11,Table5[psnr (jdf)])+1</f>
         <v>10</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <f>_xlfn.RANK.EQ(js_tests!H11,Table5[rmse (jdf)],1)</f>
         <v>10</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="8">
         <f>_xlfn.RANK.EQ(js_tests!I11,Table5[nrmse (jdf)],1)</f>
         <v>10</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="8">
         <f>_xlfn.RANK.EQ(js_tests!J11,Table5[inrmse (jdf)])</f>
         <v>10</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="8">
         <f>_xlfn.RANK.EQ(js_tests!K11,Table5[nmse (jdf)],1)</f>
         <v>10</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="8">
         <f>_xlfn.RANK.EQ(js_tests!L11,Table5[inmse (jdf)])</f>
         <v>10</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="8">
         <f>_xlfn.RANK.EQ(js_tests!M11,Table5[mse (darosh)],1)</f>
         <v>10</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="9">
         <f>_xlfn.RANK.EQ(js_tests!N11,Table5[psnr (darosh)])+1</f>
         <v>10</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="6">
         <f>_xlfn.RANK.EQ(js_tests!O11,Table5[msssim (darosh)])</f>
         <v>10</v>
       </c>
-      <c r="O13" s="12">
+      <c r="O13" s="11">
         <f>_xlfn.RANK.EQ(js_tests!P11,Table5[ssim (darosh msssim)])</f>
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.5">
-      <c r="Q14" s="20" t="s">
+      <c r="Q14" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="R14" s="27"/>
-      <c r="S14" s="27"/>
-      <c r="T14" s="27"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="27"/>
-      <c r="W14" s="27"/>
-      <c r="X14" s="23"/>
-      <c r="Y14" s="24"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="29"/>
+      <c r="V14" s="28"/>
+      <c r="W14" s="28"/>
+      <c r="X14" s="29"/>
+      <c r="Y14" s="30"/>
     </row>
     <row r="15" spans="2:25" ht="32" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="Q15" s="25" t="str">
+      <c r="Q15" s="16" t="str">
         <f>Table6[[#Headers],[Expected rank]]</f>
         <v>Expected rank</v>
       </c>
-      <c r="R15" s="28" t="str">
+      <c r="R15" s="19" t="str">
         <f>Table6[[#Headers],[mse]]</f>
         <v>mse</v>
       </c>
-      <c r="S15" s="31" t="str">
+      <c r="S15" s="21" t="str">
         <f>Table6[[#Headers],[rmse]]</f>
         <v>rmse</v>
       </c>
-      <c r="T15" s="29" t="str">
+      <c r="T15" s="20" t="str">
         <f>Table6[[#Headers],[psnr]]</f>
         <v>psnr</v>
       </c>
-      <c r="U15" s="30" t="str">
+      <c r="U15" s="18" t="str">
         <f>Table6[[#Headers],[uqi]]</f>
         <v>uqi</v>
       </c>
-      <c r="V15" s="28" t="str">
+      <c r="V15" s="19" t="str">
         <f>Table6[[#Headers],[ssim]]</f>
         <v>ssim</v>
       </c>
-      <c r="W15" s="29" t="s">
+      <c r="W15" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="X15" s="26" t="str">
+      <c r="X15" s="17" t="str">
         <f>Table6[[#Headers],[scc]]</f>
         <v>scc</v>
       </c>
-      <c r="Y15" s="16" t="str">
+      <c r="Y15" s="15" t="str">
         <f>Table6[[#Headers],[vifp]]</f>
         <v>vifp</v>
       </c>
@@ -4877,14 +7793,14 @@
         <f>_xlfn.RANK.EQ(py_tests!D2,Table6[mse],1)</f>
         <v>1</v>
       </c>
-      <c r="S16" s="5">
+      <c r="S16">
         <f>_xlfn.RANK.EQ(py_tests!E2,Table6[rmse],1)</f>
         <v>1</v>
       </c>
-      <c r="T16" s="15">
+      <c r="T16" s="14">
         <v>1</v>
       </c>
-      <c r="U16" s="5">
+      <c r="U16">
         <f>_xlfn.RANK.EQ(py_tests!G2,Table6[uqi],0)</f>
         <v>1</v>
       </c>
@@ -4892,15 +7808,15 @@
         <f>_xlfn.RANK.EQ(py_tests!H2,Table6[ssim],0)</f>
         <v>1</v>
       </c>
-      <c r="W16" s="11">
+      <c r="W16" s="10">
         <f>_xlfn.RANK.EQ(py_tests!I2,Table6[msssim],0)</f>
         <v>1</v>
       </c>
-      <c r="X16" s="11">
+      <c r="X16" s="10">
         <f>_xlfn.RANK.EQ(py_tests!J2,Table6[scc],0)</f>
         <v>1</v>
       </c>
-      <c r="Y16" s="13">
+      <c r="Y16" s="12">
         <f>_xlfn.RANK.EQ(py_tests!K2,Table6[vifp],0)</f>
         <v>1</v>
       </c>
@@ -4914,15 +7830,15 @@
         <f>_xlfn.RANK.EQ(py_tests!D3,Table6[mse],1)</f>
         <v>2</v>
       </c>
-      <c r="S17" s="5">
+      <c r="S17">
         <f>_xlfn.RANK.EQ(py_tests!E3,Table6[rmse],1)</f>
         <v>2</v>
       </c>
-      <c r="T17" s="6">
+      <c r="T17" s="5">
         <f>_xlfn.RANK.EQ(py_tests!F3,Table6[psnr],0)+1</f>
         <v>2</v>
       </c>
-      <c r="U17" s="5">
+      <c r="U17">
         <f>_xlfn.RANK.EQ(py_tests!G3,Table6[uqi],0)</f>
         <v>2</v>
       </c>
@@ -4930,15 +7846,15 @@
         <f>_xlfn.RANK.EQ(py_tests!H3,Table6[ssim],0)</f>
         <v>2</v>
       </c>
-      <c r="W17" s="11">
+      <c r="W17" s="10">
         <f>_xlfn.RANK.EQ(py_tests!I3,Table6[msssim],0)</f>
         <v>2</v>
       </c>
-      <c r="X17" s="11">
+      <c r="X17" s="10">
         <f>_xlfn.RANK.EQ(py_tests!J3,Table6[scc],0)</f>
         <v>2</v>
       </c>
-      <c r="Y17" s="13">
+      <c r="Y17" s="12">
         <f>_xlfn.RANK.EQ(py_tests!K3,Table6[vifp],0)</f>
         <v>2</v>
       </c>
@@ -4952,15 +7868,15 @@
         <f>_xlfn.RANK.EQ(py_tests!D4,Table6[mse],1)</f>
         <v>3</v>
       </c>
-      <c r="S18" s="5">
+      <c r="S18">
         <f>_xlfn.RANK.EQ(py_tests!E4,Table6[rmse],1)</f>
         <v>3</v>
       </c>
-      <c r="T18" s="6">
+      <c r="T18" s="5">
         <f>_xlfn.RANK.EQ(py_tests!F4,Table6[psnr],0)+1</f>
         <v>3</v>
       </c>
-      <c r="U18" s="5">
+      <c r="U18">
         <f>_xlfn.RANK.EQ(py_tests!G4,Table6[uqi],0)</f>
         <v>3</v>
       </c>
@@ -4968,15 +7884,15 @@
         <f>_xlfn.RANK.EQ(py_tests!H4,Table6[ssim],0)</f>
         <v>6</v>
       </c>
-      <c r="W18" s="11">
+      <c r="W18" s="10">
         <f>_xlfn.RANK.EQ(py_tests!I4,Table6[msssim],0)</f>
         <v>5</v>
       </c>
-      <c r="X18" s="11">
+      <c r="X18" s="10">
         <f>_xlfn.RANK.EQ(py_tests!J4,Table6[scc],0)</f>
         <v>7</v>
       </c>
-      <c r="Y18" s="13">
+      <c r="Y18" s="12">
         <f>_xlfn.RANK.EQ(py_tests!K4,Table6[vifp],0)</f>
         <v>5</v>
       </c>
@@ -4990,15 +7906,15 @@
         <f>_xlfn.RANK.EQ(py_tests!D5,Table6[mse],1)</f>
         <v>5</v>
       </c>
-      <c r="S19" s="5">
+      <c r="S19">
         <f>_xlfn.RANK.EQ(py_tests!E5,Table6[rmse],1)</f>
         <v>5</v>
       </c>
-      <c r="T19" s="6">
+      <c r="T19" s="5">
         <f>_xlfn.RANK.EQ(py_tests!F5,Table6[psnr],0)+1</f>
         <v>5</v>
       </c>
-      <c r="U19" s="5">
+      <c r="U19">
         <f>_xlfn.RANK.EQ(py_tests!G5,Table6[uqi],0)</f>
         <v>5</v>
       </c>
@@ -5006,15 +7922,15 @@
         <f>_xlfn.RANK.EQ(py_tests!H5,Table6[ssim],0)</f>
         <v>7</v>
       </c>
-      <c r="W19" s="11">
+      <c r="W19" s="10">
         <f>_xlfn.RANK.EQ(py_tests!I5,Table6[msssim],0)</f>
         <v>6</v>
       </c>
-      <c r="X19" s="11">
+      <c r="X19" s="10">
         <f>_xlfn.RANK.EQ(py_tests!J5,Table6[scc],0)</f>
         <v>10</v>
       </c>
-      <c r="Y19" s="13">
+      <c r="Y19" s="12">
         <f>_xlfn.RANK.EQ(py_tests!K5,Table6[vifp],0)</f>
         <v>6</v>
       </c>
@@ -5028,15 +7944,15 @@
         <f>_xlfn.RANK.EQ(py_tests!D6,Table6[mse],1)</f>
         <v>6</v>
       </c>
-      <c r="S20" s="5">
+      <c r="S20">
         <f>_xlfn.RANK.EQ(py_tests!E6,Table6[rmse],1)</f>
         <v>6</v>
       </c>
-      <c r="T20" s="6">
+      <c r="T20" s="5">
         <f>_xlfn.RANK.EQ(py_tests!F6,Table6[psnr],0)+1</f>
         <v>6</v>
       </c>
-      <c r="U20" s="5">
+      <c r="U20">
         <f>_xlfn.RANK.EQ(py_tests!G6,Table6[uqi],0)</f>
         <v>6</v>
       </c>
@@ -5044,15 +7960,15 @@
         <f>_xlfn.RANK.EQ(py_tests!H6,Table6[ssim],0)</f>
         <v>8</v>
       </c>
-      <c r="W20" s="11">
+      <c r="W20" s="10">
         <f>_xlfn.RANK.EQ(py_tests!I6,Table6[msssim],0)</f>
         <v>8</v>
       </c>
-      <c r="X20" s="11">
+      <c r="X20" s="10">
         <f>_xlfn.RANK.EQ(py_tests!J6,Table6[scc],0)</f>
         <v>9</v>
       </c>
-      <c r="Y20" s="13">
+      <c r="Y20" s="12">
         <f>_xlfn.RANK.EQ(py_tests!K6,Table6[vifp],0)</f>
         <v>7</v>
       </c>
@@ -5066,15 +7982,15 @@
         <f>_xlfn.RANK.EQ(py_tests!D7,Table6[mse],1)</f>
         <v>4</v>
       </c>
-      <c r="S21" s="5">
+      <c r="S21">
         <f>_xlfn.RANK.EQ(py_tests!E7,Table6[rmse],1)</f>
         <v>4</v>
       </c>
-      <c r="T21" s="6">
+      <c r="T21" s="5">
         <f>_xlfn.RANK.EQ(py_tests!F7,Table6[psnr],0)+1</f>
         <v>4</v>
       </c>
-      <c r="U21" s="5">
+      <c r="U21">
         <f>_xlfn.RANK.EQ(py_tests!G7,Table6[uqi],0)</f>
         <v>4</v>
       </c>
@@ -5082,15 +7998,15 @@
         <f>_xlfn.RANK.EQ(py_tests!H7,Table6[ssim],0)</f>
         <v>5</v>
       </c>
-      <c r="W21" s="11">
+      <c r="W21" s="10">
         <f>_xlfn.RANK.EQ(py_tests!I7,Table6[msssim],0)</f>
         <v>4</v>
       </c>
-      <c r="X21" s="11">
+      <c r="X21" s="10">
         <f>_xlfn.RANK.EQ(py_tests!J7,Table6[scc],0)</f>
         <v>6</v>
       </c>
-      <c r="Y21" s="13">
+      <c r="Y21" s="12">
         <f>_xlfn.RANK.EQ(py_tests!K7,Table6[vifp],0)</f>
         <v>4</v>
       </c>
@@ -5104,15 +8020,15 @@
         <f>_xlfn.RANK.EQ(py_tests!D8,Table6[mse],1)</f>
         <v>7</v>
       </c>
-      <c r="S22" s="5">
+      <c r="S22">
         <f>_xlfn.RANK.EQ(py_tests!E8,Table6[rmse],1)</f>
         <v>7</v>
       </c>
-      <c r="T22" s="6">
+      <c r="T22" s="5">
         <f>_xlfn.RANK.EQ(py_tests!F8,Table6[psnr],0)+1</f>
         <v>7</v>
       </c>
-      <c r="U22" s="5">
+      <c r="U22">
         <f>_xlfn.RANK.EQ(py_tests!G8,Table6[uqi],0)</f>
         <v>7</v>
       </c>
@@ -5120,15 +8036,15 @@
         <f>_xlfn.RANK.EQ(py_tests!H8,Table6[ssim],0)</f>
         <v>4</v>
       </c>
-      <c r="W22" s="11">
+      <c r="W22" s="10">
         <f>_xlfn.RANK.EQ(py_tests!I8,Table6[msssim],0)</f>
         <v>3</v>
       </c>
-      <c r="X22" s="11">
+      <c r="X22" s="10">
         <f>_xlfn.RANK.EQ(py_tests!J8,Table6[scc],0)</f>
         <v>8</v>
       </c>
-      <c r="Y22" s="13">
+      <c r="Y22" s="12">
         <f>_xlfn.RANK.EQ(py_tests!K8,Table6[vifp],0)</f>
         <v>3</v>
       </c>
@@ -5142,15 +8058,15 @@
         <f>_xlfn.RANK.EQ(py_tests!D9,Table6[mse],1)</f>
         <v>9</v>
       </c>
-      <c r="S23" s="5">
+      <c r="S23">
         <f>_xlfn.RANK.EQ(py_tests!E9,Table6[rmse],1)</f>
         <v>9</v>
       </c>
-      <c r="T23" s="6">
+      <c r="T23" s="5">
         <f>_xlfn.RANK.EQ(py_tests!F9,Table6[psnr],0)+1</f>
         <v>9</v>
       </c>
-      <c r="U23" s="5">
+      <c r="U23">
         <f>_xlfn.RANK.EQ(py_tests!G9,Table6[uqi],0)</f>
         <v>10</v>
       </c>
@@ -5158,15 +8074,15 @@
         <f>_xlfn.RANK.EQ(py_tests!H9,Table6[ssim],0)</f>
         <v>3</v>
       </c>
-      <c r="W23" s="11">
+      <c r="W23" s="10">
         <f>_xlfn.RANK.EQ(py_tests!I9,Table6[msssim],0)</f>
         <v>7</v>
       </c>
-      <c r="X23" s="11">
+      <c r="X23" s="10">
         <f>_xlfn.RANK.EQ(py_tests!J9,Table6[scc],0)</f>
         <v>5</v>
       </c>
-      <c r="Y23" s="13">
+      <c r="Y23" s="12">
         <f>_xlfn.RANK.EQ(py_tests!K9,Table6[vifp],0)</f>
         <v>8</v>
       </c>
@@ -5180,15 +8096,15 @@
         <f>_xlfn.RANK.EQ(py_tests!D10,Table6[mse],1)</f>
         <v>8</v>
       </c>
-      <c r="S24" s="5">
+      <c r="S24">
         <f>_xlfn.RANK.EQ(py_tests!E10,Table6[rmse],1)</f>
         <v>8</v>
       </c>
-      <c r="T24" s="6">
+      <c r="T24" s="5">
         <f>_xlfn.RANK.EQ(py_tests!F10,Table6[psnr],0)+1</f>
         <v>8</v>
       </c>
-      <c r="U24" s="5">
+      <c r="U24">
         <f>_xlfn.RANK.EQ(py_tests!G10,Table6[uqi],0)</f>
         <v>8</v>
       </c>
@@ -5196,53 +8112,53 @@
         <f>_xlfn.RANK.EQ(py_tests!H10,Table6[ssim],0)</f>
         <v>9</v>
       </c>
-      <c r="W24" s="11">
+      <c r="W24" s="10">
         <f>_xlfn.RANK.EQ(py_tests!I10,Table6[msssim],0)</f>
         <v>9</v>
       </c>
-      <c r="X24" s="11">
+      <c r="X24" s="10">
         <f>_xlfn.RANK.EQ(py_tests!J10,Table6[scc],0)</f>
         <v>4</v>
       </c>
-      <c r="Y24" s="13">
+      <c r="Y24" s="12">
         <f>_xlfn.RANK.EQ(py_tests!K10,Table6[vifp],0)</f>
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="17:25" x14ac:dyDescent="0.5">
-      <c r="Q25" s="7">
+      <c r="Q25" s="6">
         <f>py_tests!C11</f>
         <v>10</v>
       </c>
-      <c r="R25" s="7">
+      <c r="R25" s="6">
         <f>_xlfn.RANK.EQ(py_tests!D11,Table6[mse],1)</f>
         <v>10</v>
       </c>
-      <c r="S25" s="9">
+      <c r="S25" s="8">
         <f>_xlfn.RANK.EQ(py_tests!E11,Table6[rmse],1)</f>
         <v>10</v>
       </c>
-      <c r="T25" s="10">
+      <c r="T25" s="9">
         <f>_xlfn.RANK.EQ(py_tests!F11,Table6[psnr],0)+1</f>
         <v>10</v>
       </c>
-      <c r="U25" s="9">
+      <c r="U25" s="8">
         <f>_xlfn.RANK.EQ(py_tests!G11,Table6[uqi],0)</f>
         <v>9</v>
       </c>
-      <c r="V25" s="7">
+      <c r="V25" s="6">
         <f>_xlfn.RANK.EQ(py_tests!H11,Table6[ssim],0)</f>
         <v>10</v>
       </c>
-      <c r="W25" s="12">
+      <c r="W25" s="11">
         <f>_xlfn.RANK.EQ(py_tests!I11,Table6[msssim],0)</f>
         <v>10</v>
       </c>
-      <c r="X25" s="12">
+      <c r="X25" s="11">
         <f>_xlfn.RANK.EQ(py_tests!J11,Table6[scc],0)</f>
         <v>3</v>
       </c>
-      <c r="Y25" s="14">
+      <c r="Y25" s="13">
         <f>_xlfn.RANK.EQ(py_tests!K11,Table6[vifp],0)</f>
         <v>10</v>
       </c>
@@ -5256,12 +8172,12 @@
     <mergeCell ref="Q14:Y14"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:O13">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$B4&lt;&gt;C4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R16:Y25">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$Q16&lt;&gt;R16</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>